<commit_message>
Add Financial data and functions. Finished dividend scripts and notebooks.
</commit_message>
<xml_diff>
--- a/dashboards/Dashboard_CashFlow.xlsx
+++ b/dashboards/Dashboard_CashFlow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/telamon/DataScience/repositories/investing/dashboards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22FD402E-712A-3B43-A7A6-0017282CDF54}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BADEAF-4F4A-4646-ADB1-8161EE368B13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1355,22 +1355,22 @@
             <v>CashFlow</v>
           </cell>
           <cell r="D2">
-            <v>20</v>
+            <v>15</v>
           </cell>
           <cell r="E2">
-            <v>15</v>
+            <v>10</v>
           </cell>
           <cell r="F2">
-            <v>15</v>
+            <v>5</v>
           </cell>
           <cell r="G2">
-            <v>10</v>
+            <v>14</v>
           </cell>
           <cell r="H2">
-            <v>10</v>
+            <v>9</v>
           </cell>
           <cell r="I2">
-            <v>5</v>
+            <v>4</v>
           </cell>
           <cell r="J2">
             <v>6</v>
@@ -1391,16 +1391,16 @@
             <v>10</v>
           </cell>
           <cell r="P2">
-            <v>284.81945398417798</v>
+            <v>184.34308241546901</v>
           </cell>
           <cell r="Q2">
-            <v>120.576607366093</v>
+            <v>91.470527693796996</v>
           </cell>
           <cell r="R2">
-            <v>56.279269215865597</v>
+            <v>51.255174279427401</v>
           </cell>
           <cell r="S2">
-            <v>150.56025990645</v>
+            <v>107.267688085987</v>
           </cell>
         </row>
         <row r="3">
@@ -1417,19 +1417,19 @@
             <v>10</v>
           </cell>
           <cell r="E3">
+            <v>7</v>
+          </cell>
+          <cell r="F3">
+            <v>4</v>
+          </cell>
+          <cell r="G3">
             <v>9</v>
-          </cell>
-          <cell r="F3">
-            <v>8</v>
-          </cell>
-          <cell r="G3">
-            <v>7</v>
           </cell>
           <cell r="H3">
             <v>6</v>
           </cell>
           <cell r="I3">
-            <v>5</v>
+            <v>3</v>
           </cell>
           <cell r="J3">
             <v>6</v>
@@ -1450,16 +1450,16 @@
             <v>10</v>
           </cell>
           <cell r="P3">
-            <v>334.94598944940702</v>
+            <v>305.32416689419199</v>
           </cell>
           <cell r="Q3">
-            <v>182.201835350072</v>
+            <v>165.50620010220399</v>
           </cell>
           <cell r="R3">
-            <v>111.07568470541101</v>
+            <v>100.892440467347</v>
           </cell>
           <cell r="S3">
-            <v>206.68723638647401</v>
+            <v>188.06746224934301</v>
           </cell>
         </row>
         <row r="4">
@@ -1473,22 +1473,22 @@
             <v>CashFlow</v>
           </cell>
           <cell r="D4">
-            <v>20</v>
+            <v>25</v>
           </cell>
           <cell r="E4">
             <v>15</v>
           </cell>
           <cell r="F4">
-            <v>15</v>
+            <v>5</v>
           </cell>
           <cell r="G4">
-            <v>10</v>
+            <v>23</v>
           </cell>
           <cell r="H4">
-            <v>10</v>
+            <v>13</v>
           </cell>
           <cell r="I4">
-            <v>5</v>
+            <v>3</v>
           </cell>
           <cell r="J4">
             <v>6</v>
@@ -1509,16 +1509,16 @@
             <v>10</v>
           </cell>
           <cell r="P4">
-            <v>1534.03655646774</v>
+            <v>1881.39308684616</v>
           </cell>
           <cell r="Q4">
-            <v>649.42517432366003</v>
+            <v>720.35826699548295</v>
           </cell>
           <cell r="R4">
-            <v>303.11994191668998</v>
+            <v>314.979963873646</v>
           </cell>
           <cell r="S4">
-            <v>810.91701924479605</v>
+            <v>947.05522201413703</v>
           </cell>
         </row>
         <row r="5">
@@ -1532,22 +1532,22 @@
             <v>CashFlow</v>
           </cell>
           <cell r="D5">
-            <v>20</v>
+            <v>25</v>
           </cell>
           <cell r="E5">
             <v>15</v>
           </cell>
           <cell r="F5">
-            <v>15</v>
+            <v>5</v>
           </cell>
           <cell r="G5">
-            <v>10</v>
+            <v>23</v>
           </cell>
           <cell r="H5">
-            <v>10</v>
+            <v>13</v>
           </cell>
           <cell r="I5">
-            <v>5</v>
+            <v>3</v>
           </cell>
           <cell r="J5">
             <v>6</v>
@@ -1568,16 +1568,16 @@
             <v>10</v>
           </cell>
           <cell r="P5">
-            <v>545.605668583696</v>
+            <v>669.148807888286</v>
           </cell>
           <cell r="Q5">
-            <v>230.978887001115</v>
+            <v>256.20742362805998</v>
           </cell>
           <cell r="R5">
-            <v>107.809659341703</v>
+            <v>112.027873817726</v>
           </cell>
           <cell r="S5">
-            <v>288.416153178066</v>
+            <v>336.83597396302798</v>
           </cell>
         </row>
         <row r="6">
@@ -1591,19 +1591,19 @@
             <v>CashFlow</v>
           </cell>
           <cell r="D6">
-            <v>12</v>
+            <v>10</v>
           </cell>
           <cell r="E6">
-            <v>11</v>
+            <v>7</v>
           </cell>
           <cell r="F6">
-            <v>8</v>
+            <v>4</v>
           </cell>
           <cell r="G6">
-            <v>7</v>
+            <v>9</v>
           </cell>
           <cell r="H6">
-            <v>4</v>
+            <v>6</v>
           </cell>
           <cell r="I6">
             <v>3</v>
@@ -1627,16 +1627,16 @@
             <v>10</v>
           </cell>
           <cell r="P6">
-            <v>367.72795745525201</v>
+            <v>279.70740005726498</v>
           </cell>
           <cell r="Q6">
-            <v>166.91506004859201</v>
+            <v>151.62019238387799</v>
           </cell>
           <cell r="R6">
-            <v>84.030853180782202</v>
+            <v>92.427541834032496</v>
           </cell>
           <cell r="S6">
-            <v>202.29366721024701</v>
+            <v>172.28855952094</v>
           </cell>
         </row>
         <row r="7">
@@ -1656,16 +1656,16 @@
             <v>10</v>
           </cell>
           <cell r="F7">
-            <v>10</v>
+            <v>5</v>
           </cell>
           <cell r="G7">
-            <v>5</v>
+            <v>13</v>
           </cell>
           <cell r="H7">
-            <v>5</v>
+            <v>8</v>
           </cell>
           <cell r="I7">
-            <v>0</v>
+            <v>3</v>
           </cell>
           <cell r="J7">
             <v>6</v>
@@ -1689,13 +1689,13 @@
             <v>639.73999696427597</v>
           </cell>
           <cell r="Q7">
-            <v>265.519861278414</v>
+            <v>303.756656725016</v>
           </cell>
           <cell r="R7">
-            <v>121.272319063518</v>
+            <v>161.852752007102</v>
           </cell>
           <cell r="S7">
-            <v>334.51163931970399</v>
+            <v>361.98048738142001</v>
           </cell>
         </row>
         <row r="8">
@@ -1709,22 +1709,22 @@
             <v>CashFlow</v>
           </cell>
           <cell r="D8">
-            <v>20</v>
+            <v>7</v>
           </cell>
           <cell r="E8">
-            <v>15</v>
+            <v>5</v>
           </cell>
           <cell r="F8">
-            <v>15</v>
+            <v>3</v>
           </cell>
           <cell r="G8">
-            <v>10</v>
+            <v>6</v>
           </cell>
           <cell r="H8">
-            <v>10</v>
+            <v>4</v>
           </cell>
           <cell r="I8">
-            <v>5</v>
+            <v>2</v>
           </cell>
           <cell r="J8">
             <v>6</v>
@@ -1745,16 +1745,16 @@
             <v>10</v>
           </cell>
           <cell r="P8">
-            <v>173.34613088085499</v>
+            <v>61.998917149226799</v>
           </cell>
           <cell r="Q8">
-            <v>73.385044698573594</v>
+            <v>35.145553343478603</v>
           </cell>
           <cell r="R8">
-            <v>34.252553436585998</v>
+            <v>22.3846643508112</v>
           </cell>
           <cell r="S8">
-            <v>91.633623174662006</v>
+            <v>39.373295787402803</v>
           </cell>
         </row>
         <row r="9">
@@ -1774,16 +1774,16 @@
             <v>15</v>
           </cell>
           <cell r="F9">
-            <v>15</v>
+            <v>10</v>
           </cell>
           <cell r="G9">
-            <v>10</v>
+            <v>18</v>
           </cell>
           <cell r="H9">
-            <v>10</v>
+            <v>13</v>
           </cell>
           <cell r="I9">
-            <v>5</v>
+            <v>8</v>
           </cell>
           <cell r="J9">
             <v>6</v>
@@ -1807,13 +1807,13 @@
             <v>5132.3749724222598</v>
           </cell>
           <cell r="Q9">
-            <v>2172.7601582288598</v>
+            <v>2471.34071290063</v>
           </cell>
           <cell r="R9">
-            <v>1014.1382856726</v>
+            <v>1335.66717251144</v>
           </cell>
           <cell r="S9">
-            <v>2713.05804072</v>
+            <v>2928.94892864036</v>
           </cell>
         </row>
         <row r="10">
@@ -1827,22 +1827,22 @@
             <v>CashFlow</v>
           </cell>
           <cell r="D10">
-            <v>11</v>
+            <v>0</v>
           </cell>
           <cell r="E10">
-            <v>9</v>
+            <v>0</v>
           </cell>
           <cell r="F10">
-            <v>9</v>
+            <v>0</v>
           </cell>
           <cell r="G10">
-            <v>7</v>
+            <v>0</v>
           </cell>
           <cell r="H10">
-            <v>7</v>
+            <v>0</v>
           </cell>
           <cell r="I10">
-            <v>5</v>
+            <v>0</v>
           </cell>
           <cell r="J10">
             <v>6</v>
@@ -1863,16 +1863,16 @@
             <v>10</v>
           </cell>
           <cell r="P10">
-            <v>-5.2978102793225803</v>
+            <v>-2.0433794339765101</v>
           </cell>
           <cell r="Q10">
-            <v>-2.88427463790243</v>
+            <v>-1.33655007002237</v>
           </cell>
           <cell r="R10">
-            <v>-1.7598624002953001</v>
+            <v>-0.98313538804530498</v>
           </cell>
           <cell r="S10">
-            <v>-3.2710116590463398</v>
+            <v>-1.44257447461549</v>
           </cell>
         </row>
         <row r="11">
@@ -1892,16 +1892,16 @@
             <v>15</v>
           </cell>
           <cell r="F11">
-            <v>15</v>
+            <v>10</v>
           </cell>
           <cell r="G11">
-            <v>10</v>
+            <v>17</v>
           </cell>
           <cell r="H11">
-            <v>10</v>
+            <v>12</v>
           </cell>
           <cell r="I11">
-            <v>5</v>
+            <v>7</v>
           </cell>
           <cell r="J11">
             <v>6</v>
@@ -1925,13 +1925,13 @@
             <v>447.42732896976003</v>
           </cell>
           <cell r="Q11">
-            <v>189.41567584440099</v>
+            <v>206.469556484902</v>
           </cell>
           <cell r="R11">
-            <v>88.409983059034801</v>
+            <v>106.31643073057</v>
           </cell>
           <cell r="S11">
-            <v>236.517463946399</v>
+            <v>248.71095050406001</v>
           </cell>
         </row>
         <row r="12">
@@ -1948,19 +1948,19 @@
             <v>25</v>
           </cell>
           <cell r="E12">
-            <v>20</v>
+            <v>10</v>
           </cell>
           <cell r="F12">
-            <v>10</v>
+            <v>0</v>
           </cell>
           <cell r="G12">
-            <v>5</v>
+            <v>23</v>
           </cell>
           <cell r="H12">
-            <v>-5</v>
+            <v>8</v>
           </cell>
           <cell r="I12">
-            <v>-5</v>
+            <v>-2</v>
           </cell>
           <cell r="J12">
             <v>6</v>
@@ -1981,16 +1981,16 @@
             <v>10</v>
           </cell>
           <cell r="P12">
-            <v>553.953778990302</v>
+            <v>358.53431254889699</v>
           </cell>
           <cell r="Q12">
-            <v>98.076141206822598</v>
+            <v>134.33185323863401</v>
           </cell>
           <cell r="R12">
-            <v>21.0144291894979</v>
+            <v>46.615537998802701</v>
           </cell>
           <cell r="S12">
-            <v>211.72091893666899</v>
+            <v>175.27769645976301</v>
           </cell>
         </row>
         <row r="13">
@@ -2004,22 +2004,22 @@
             <v>CashFlow</v>
           </cell>
           <cell r="D13">
-            <v>20</v>
+            <v>10</v>
           </cell>
           <cell r="E13">
-            <v>15</v>
+            <v>7</v>
           </cell>
           <cell r="F13">
-            <v>15</v>
+            <v>4</v>
           </cell>
           <cell r="G13">
-            <v>10</v>
+            <v>8</v>
           </cell>
           <cell r="H13">
-            <v>10</v>
+            <v>5</v>
           </cell>
           <cell r="I13">
-            <v>5</v>
+            <v>2</v>
           </cell>
           <cell r="J13">
             <v>6</v>
@@ -2040,16 +2040,16 @@
             <v>10</v>
           </cell>
           <cell r="P13">
-            <v>380.44106600400198</v>
+            <v>171.70157231237999</v>
           </cell>
           <cell r="Q13">
-            <v>161.05744323226699</v>
+            <v>88.8819648768349</v>
           </cell>
           <cell r="R13">
-            <v>75.173745595339298</v>
+            <v>51.535159307582497</v>
           </cell>
           <cell r="S13">
-            <v>201.10742077270899</v>
+            <v>102.523805436722</v>
           </cell>
         </row>
         <row r="14">
@@ -2063,22 +2063,22 @@
             <v>CashFlow</v>
           </cell>
           <cell r="D14">
-            <v>25</v>
+            <v>10</v>
           </cell>
           <cell r="E14">
-            <v>10</v>
+            <v>7</v>
           </cell>
           <cell r="F14">
-            <v>6</v>
+            <v>4</v>
           </cell>
           <cell r="G14">
-            <v>6</v>
+            <v>8</v>
           </cell>
           <cell r="H14">
-            <v>-5</v>
+            <v>5</v>
           </cell>
           <cell r="I14">
-            <v>-5</v>
+            <v>2</v>
           </cell>
           <cell r="J14">
             <v>6</v>
@@ -2099,16 +2099,16 @@
             <v>10</v>
           </cell>
           <cell r="P14">
-            <v>32.639678313274899</v>
+            <v>15.000809409011699</v>
           </cell>
           <cell r="Q14">
-            <v>7.7790622461947203</v>
+            <v>7.7652254260675599</v>
           </cell>
           <cell r="R14">
-            <v>1.91307828755934</v>
+            <v>4.5023996706893303</v>
           </cell>
           <cell r="S14">
-            <v>13.4774518787281</v>
+            <v>8.9570528943373393</v>
           </cell>
         </row>
         <row r="15">
@@ -2122,22 +2122,22 @@
             <v>CashFlow</v>
           </cell>
           <cell r="D15">
-            <v>20</v>
+            <v>10</v>
           </cell>
           <cell r="E15">
-            <v>15</v>
+            <v>7</v>
           </cell>
           <cell r="F15">
-            <v>15</v>
+            <v>4</v>
           </cell>
           <cell r="G15">
-            <v>10</v>
+            <v>8</v>
           </cell>
           <cell r="H15">
-            <v>10</v>
+            <v>5</v>
           </cell>
           <cell r="I15">
-            <v>5</v>
+            <v>2</v>
           </cell>
           <cell r="J15">
             <v>6</v>
@@ -2158,16 +2158,16 @@
             <v>10</v>
           </cell>
           <cell r="P15">
-            <v>404.98565090748502</v>
+            <v>182.779093106727</v>
           </cell>
           <cell r="Q15">
-            <v>171.44824602144601</v>
+            <v>94.616285191469402</v>
           </cell>
           <cell r="R15">
-            <v>80.023664666006297</v>
+            <v>54.860008295168399</v>
           </cell>
           <cell r="S15">
-            <v>214.08209308062601</v>
+            <v>109.13824449715599</v>
           </cell>
         </row>
         <row r="16">
@@ -2181,22 +2181,22 @@
             <v>CashFlow</v>
           </cell>
           <cell r="D16">
-            <v>20</v>
+            <v>15</v>
           </cell>
           <cell r="E16">
-            <v>15</v>
+            <v>10</v>
           </cell>
           <cell r="F16">
-            <v>15</v>
+            <v>5</v>
           </cell>
           <cell r="G16">
-            <v>10</v>
+            <v>14</v>
           </cell>
           <cell r="H16">
-            <v>10</v>
+            <v>9</v>
           </cell>
           <cell r="I16">
-            <v>5</v>
+            <v>4</v>
           </cell>
           <cell r="J16">
             <v>6</v>
@@ -2217,16 +2217,16 @@
             <v>10</v>
           </cell>
           <cell r="P16">
-            <v>236.75297521485601</v>
+            <v>153.233118776233</v>
           </cell>
           <cell r="Q16">
-            <v>100.22795190395099</v>
+            <v>76.033849770606807</v>
           </cell>
           <cell r="R16">
-            <v>46.781511035809203</v>
+            <v>42.605288494389399</v>
           </cell>
           <cell r="S16">
-            <v>125.15152663678001</v>
+            <v>89.165062089429696</v>
           </cell>
         </row>
         <row r="17">
@@ -2243,13 +2243,13 @@
             <v>6</v>
           </cell>
           <cell r="E17">
-            <v>5</v>
+            <v>4</v>
           </cell>
           <cell r="F17">
+            <v>3</v>
+          </cell>
+          <cell r="G17">
             <v>4</v>
-          </cell>
-          <cell r="G17">
-            <v>3</v>
           </cell>
           <cell r="H17">
             <v>2</v>
@@ -2276,7 +2276,7 @@
             <v>10</v>
           </cell>
           <cell r="P17">
-            <v>21.812470504449099</v>
+            <v>20.793378457782499</v>
           </cell>
           <cell r="Q17">
             <v>11.781974280616099</v>
@@ -2285,7 +2285,7 @@
             <v>7.1301895264458901</v>
           </cell>
           <cell r="S17">
-            <v>13.3955877215149</v>
+            <v>13.0898601075149</v>
           </cell>
         </row>
         <row r="18">
@@ -2299,22 +2299,22 @@
             <v>CashFlow</v>
           </cell>
           <cell r="D18">
-            <v>18</v>
+            <v>12</v>
           </cell>
           <cell r="E18">
-            <v>15</v>
+            <v>8</v>
           </cell>
           <cell r="F18">
-            <v>13</v>
+            <v>4</v>
           </cell>
           <cell r="G18">
-            <v>10</v>
+            <v>11</v>
           </cell>
           <cell r="H18">
-            <v>8</v>
+            <v>7</v>
           </cell>
           <cell r="I18">
-            <v>5</v>
+            <v>3</v>
           </cell>
           <cell r="J18">
             <v>6</v>
@@ -2335,16 +2335,16 @@
             <v>10</v>
           </cell>
           <cell r="P18">
-            <v>909.23203828066505</v>
+            <v>511.66343592989801</v>
           </cell>
           <cell r="Q18">
-            <v>383.50175019474602</v>
+            <v>264.96792059043599</v>
           </cell>
           <cell r="R18">
-            <v>178.28100586497601</v>
+            <v>154.57697883830301</v>
           </cell>
           <cell r="S18">
-            <v>479.654613321591</v>
+            <v>305.85929266663499</v>
           </cell>
         </row>
         <row r="19">
@@ -2361,19 +2361,19 @@
             <v>25</v>
           </cell>
           <cell r="E19">
+            <v>20</v>
+          </cell>
+          <cell r="F19">
             <v>15</v>
           </cell>
-          <cell r="F19">
+          <cell r="G19">
+            <v>22</v>
+          </cell>
+          <cell r="H19">
             <v>17</v>
           </cell>
-          <cell r="G19">
-            <v>10</v>
-          </cell>
-          <cell r="H19">
-            <v>10</v>
-          </cell>
           <cell r="I19">
-            <v>5</v>
+            <v>12</v>
           </cell>
           <cell r="J19">
             <v>6</v>
@@ -2394,16 +2394,16 @@
             <v>10</v>
           </cell>
           <cell r="P19">
-            <v>427.70336174302798</v>
+            <v>529.12671886748706</v>
           </cell>
           <cell r="Q19">
-            <v>160.92827145451801</v>
+            <v>247.75816005735601</v>
           </cell>
           <cell r="R19">
-            <v>68.909266795727703</v>
+            <v>129.53500014332499</v>
           </cell>
           <cell r="S19">
-            <v>213.35509714343399</v>
+            <v>296.70177972618598</v>
           </cell>
         </row>
       </sheetData>
@@ -2789,11 +2789,11 @@
       </c>
       <c r="E3">
         <f>VLOOKUP(A3,NPV!$A$2:$S$20,19,FALSE)</f>
-        <v>150.56025990645</v>
+        <v>107.267688085987</v>
       </c>
       <c r="F3" s="2">
         <f t="shared" ref="F3:F38" si="0">D3/E3</f>
-        <v>1.0906596921119704</v>
+        <v>1.5308431611039699</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2815,11 +2815,11 @@
       </c>
       <c r="E4">
         <f>VLOOKUP(A4,NPV!$A$2:$S$20,19,FALSE)</f>
-        <v>206.68723638647401</v>
+        <v>188.06746224934301</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" si="0"/>
-        <v>1.5275738188107582</v>
+        <v>1.6788125240278291</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2867,11 +2867,11 @@
       </c>
       <c r="E6">
         <f>VLOOKUP(A6,NPV!$A$2:$S$20,19,FALSE)</f>
-        <v>810.91701924479605</v>
+        <v>947.05522201413703</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" si="0"/>
-        <v>3.7687702188758601</v>
+        <v>3.2270134212551227</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2945,11 +2945,11 @@
       </c>
       <c r="E9">
         <f>VLOOKUP(A9,NPV!$A$2:$S$20,19,FALSE)</f>
-        <v>288.416153178066</v>
+        <v>336.83597396302798</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="0"/>
-        <v>0.36849393100796529</v>
+        <v>0.31552331183737081</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -3205,11 +3205,11 @@
       </c>
       <c r="E19">
         <f>VLOOKUP(A19,NPV!$A$2:$S$20,19,FALSE)</f>
-        <v>202.29366721024701</v>
+        <v>172.28855952094</v>
       </c>
       <c r="F19" s="2">
         <f t="shared" si="0"/>
-        <v>2.5498574149042343</v>
+        <v>2.9939306983498519</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -3257,11 +3257,11 @@
       </c>
       <c r="E21">
         <f>VLOOKUP(A21,NPV!$A$2:$S$20,19,FALSE)</f>
-        <v>334.51163931970399</v>
+        <v>361.98048738142001</v>
       </c>
       <c r="F21" s="2">
         <f t="shared" si="0"/>
-        <v>0.3677599885410614</v>
+        <v>0.33985256369202971</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -3283,11 +3283,11 @@
       </c>
       <c r="E22">
         <f>VLOOKUP(A22,NPV!$A$2:$S$20,19,FALSE)</f>
-        <v>91.633623174662006</v>
+        <v>39.373295787402803</v>
       </c>
       <c r="F22" s="2">
         <f t="shared" si="0"/>
-        <v>0.59399594187634797</v>
+        <v>1.3824090469609653</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -3413,11 +3413,11 @@
       </c>
       <c r="E27">
         <f>VLOOKUP(A27,NPV!$A$2:$S$20,19,FALSE)</f>
-        <v>2713.05804072</v>
+        <v>2928.94892864036</v>
       </c>
       <c r="F27" s="2">
         <f t="shared" si="0"/>
-        <v>0.9915969247202947</v>
+        <v>0.9185069713777696</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -3439,11 +3439,11 @@
       </c>
       <c r="E28">
         <f>VLOOKUP(A28,NPV!$A$2:$S$20,19,FALSE)</f>
-        <v>-3.2710116590463398</v>
+        <v>-1.44257447461549</v>
       </c>
       <c r="F28" s="2">
         <f t="shared" si="0"/>
-        <v>-45.417140947123841</v>
+        <v>-102.98254972117874</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -3491,11 +3491,11 @@
       </c>
       <c r="E30">
         <f>VLOOKUP(A30,NPV!$A$2:$S$20,19,FALSE)</f>
-        <v>236.517463946399</v>
+        <v>248.71095050406001</v>
       </c>
       <c r="F30" s="2">
         <f t="shared" si="0"/>
-        <v>1.5346858744798173</v>
+        <v>1.4594452325105913</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -3517,11 +3517,11 @@
       </c>
       <c r="E31">
         <f>VLOOKUP(A31,NPV!$A$2:$S$20,19,FALSE)</f>
-        <v>211.72091893666899</v>
+        <v>175.27769645976301</v>
       </c>
       <c r="F31" s="2">
         <f t="shared" si="0"/>
-        <v>5.351573404994622</v>
+        <v>6.4642567876432713</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -3595,11 +3595,11 @@
       </c>
       <c r="E34">
         <f>VLOOKUP(A34,NPV!$A$2:$S$20,19,FALSE)</f>
-        <v>201.10742077270899</v>
+        <v>102.523805436722</v>
       </c>
       <c r="F34" s="2">
         <f t="shared" si="0"/>
-        <v>1.4717010445636785</v>
+        <v>2.8868417433390783</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -3621,11 +3621,11 @@
       </c>
       <c r="E35">
         <f>VLOOKUP(A35,NPV!$A$2:$S$20,19,FALSE)</f>
-        <v>13.4774518787281</v>
+        <v>8.9570528943373393</v>
       </c>
       <c r="F35" s="2">
         <f t="shared" si="0"/>
-        <v>1.408278041948942</v>
+        <v>2.1190004978351173</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -3647,11 +3647,11 @@
       </c>
       <c r="E36">
         <f>VLOOKUP(A36,NPV!$A$2:$S$20,19,FALSE)</f>
-        <v>214.08209308062601</v>
+        <v>109.13824449715599</v>
       </c>
       <c r="F36" s="2">
         <f t="shared" si="0"/>
-        <v>0.88610866148808898</v>
+        <v>1.7381624362959707</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -3673,11 +3673,11 @@
       </c>
       <c r="E37">
         <f>VLOOKUP(A37,NPV!$A$2:$S$20,19,FALSE)</f>
-        <v>125.15152663678001</v>
+        <v>89.165062089429696</v>
       </c>
       <c r="F37" s="2">
         <f t="shared" si="0"/>
-        <v>0.89163911409367902</v>
+        <v>1.2514991154940127</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -3725,11 +3725,11 @@
       </c>
       <c r="E39">
         <f>VLOOKUP(A39,NPV!$A$2:$S$20,19,FALSE)</f>
-        <v>13.3955877215149</v>
+        <v>13.0898601075149</v>
       </c>
       <c r="F39" s="2">
         <f t="shared" ref="F39:F47" si="1">D39/E39</f>
-        <v>8.4438251580916415</v>
+        <v>8.64103968119678</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -3829,11 +3829,11 @@
       </c>
       <c r="E43">
         <f>VLOOKUP(A43,NPV!$A$2:$S$20,19,FALSE)</f>
-        <v>479.654613321591</v>
+        <v>305.85929266663499</v>
       </c>
       <c r="F43" s="2">
         <f t="shared" si="1"/>
-        <v>1.3930857613977063</v>
+        <v>2.1846647403821788</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -3907,11 +3907,11 @@
       </c>
       <c r="E46">
         <f>VLOOKUP(A46,NPV!$A$2:$S$20,19,FALSE)</f>
-        <v>213.35509714343399</v>
+        <v>296.70177972618598</v>
       </c>
       <c r="F46" s="2">
         <f t="shared" si="1"/>
-        <v>1.017318104689287</v>
+        <v>0.73154263938714359</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -4920,27 +4920,27 @@
       </c>
       <c r="D2">
         <f>[2]npv!D2</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E2">
         <f>[2]npv!E2</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F2">
         <f>[2]npv!F2</f>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G2">
         <f>[2]npv!G2</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H2">
         <f>[2]npv!H2</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I2">
         <f>[2]npv!I2</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J2">
         <f>[2]npv!J2</f>
@@ -4968,19 +4968,19 @@
       </c>
       <c r="P2">
         <f>[2]npv!P2</f>
-        <v>284.81945398417798</v>
+        <v>184.34308241546901</v>
       </c>
       <c r="Q2">
         <f>[2]npv!Q2</f>
-        <v>120.576607366093</v>
+        <v>91.470527693796996</v>
       </c>
       <c r="R2">
         <f>[2]npv!R2</f>
-        <v>56.279269215865597</v>
+        <v>51.255174279427401</v>
       </c>
       <c r="S2">
         <f>[2]npv!S2</f>
-        <v>150.56025990645</v>
+        <v>107.267688085987</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -5002,15 +5002,15 @@
       </c>
       <c r="E3">
         <f>[2]npv!E3</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F3">
         <f>[2]npv!F3</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G3">
         <f>[2]npv!G3</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H3">
         <f>[2]npv!H3</f>
@@ -5018,7 +5018,7 @@
       </c>
       <c r="I3">
         <f>[2]npv!I3</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J3">
         <f>[2]npv!J3</f>
@@ -5046,19 +5046,19 @@
       </c>
       <c r="P3">
         <f>[2]npv!P3</f>
-        <v>334.94598944940702</v>
+        <v>305.32416689419199</v>
       </c>
       <c r="Q3">
         <f>[2]npv!Q3</f>
-        <v>182.201835350072</v>
+        <v>165.50620010220399</v>
       </c>
       <c r="R3">
         <f>[2]npv!R3</f>
-        <v>111.07568470541101</v>
+        <v>100.892440467347</v>
       </c>
       <c r="S3">
         <f>[2]npv!S3</f>
-        <v>206.68723638647401</v>
+        <v>188.06746224934301</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -5076,7 +5076,7 @@
       </c>
       <c r="D4">
         <f>[2]npv!D4</f>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E4">
         <f>[2]npv!E4</f>
@@ -5084,19 +5084,19 @@
       </c>
       <c r="F4">
         <f>[2]npv!F4</f>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G4">
         <f>[2]npv!G4</f>
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="H4">
         <f>[2]npv!H4</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="I4">
         <f>[2]npv!I4</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J4">
         <f>[2]npv!J4</f>
@@ -5124,19 +5124,19 @@
       </c>
       <c r="P4">
         <f>[2]npv!P4</f>
-        <v>1534.03655646774</v>
+        <v>1881.39308684616</v>
       </c>
       <c r="Q4">
         <f>[2]npv!Q4</f>
-        <v>649.42517432366003</v>
+        <v>720.35826699548295</v>
       </c>
       <c r="R4">
         <f>[2]npv!R4</f>
-        <v>303.11994191668998</v>
+        <v>314.979963873646</v>
       </c>
       <c r="S4">
         <f>[2]npv!S4</f>
-        <v>810.91701924479605</v>
+        <v>947.05522201413703</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -5154,7 +5154,7 @@
       </c>
       <c r="D5">
         <f>[2]npv!D5</f>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E5">
         <f>[2]npv!E5</f>
@@ -5162,19 +5162,19 @@
       </c>
       <c r="F5">
         <f>[2]npv!F5</f>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G5">
         <f>[2]npv!G5</f>
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="H5">
         <f>[2]npv!H5</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="I5">
         <f>[2]npv!I5</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J5">
         <f>[2]npv!J5</f>
@@ -5202,19 +5202,19 @@
       </c>
       <c r="P5">
         <f>[2]npv!P5</f>
-        <v>545.605668583696</v>
+        <v>669.148807888286</v>
       </c>
       <c r="Q5">
         <f>[2]npv!Q5</f>
-        <v>230.978887001115</v>
+        <v>256.20742362805998</v>
       </c>
       <c r="R5">
         <f>[2]npv!R5</f>
-        <v>107.809659341703</v>
+        <v>112.027873817726</v>
       </c>
       <c r="S5">
         <f>[2]npv!S5</f>
-        <v>288.416153178066</v>
+        <v>336.83597396302798</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -5232,23 +5232,23 @@
       </c>
       <c r="D6">
         <f>[2]npv!D6</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E6">
         <f>[2]npv!E6</f>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F6">
         <f>[2]npv!F6</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G6">
         <f>[2]npv!G6</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H6">
         <f>[2]npv!H6</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I6">
         <f>[2]npv!I6</f>
@@ -5280,19 +5280,19 @@
       </c>
       <c r="P6">
         <f>[2]npv!P6</f>
-        <v>367.72795745525201</v>
+        <v>279.70740005726498</v>
       </c>
       <c r="Q6">
         <f>[2]npv!Q6</f>
-        <v>166.91506004859201</v>
+        <v>151.62019238387799</v>
       </c>
       <c r="R6">
         <f>[2]npv!R6</f>
-        <v>84.030853180782202</v>
+        <v>92.427541834032496</v>
       </c>
       <c r="S6">
         <f>[2]npv!S6</f>
-        <v>202.29366721024701</v>
+        <v>172.28855952094</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -5318,19 +5318,19 @@
       </c>
       <c r="F7">
         <f>[2]npv!F7</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G7">
         <f>[2]npv!G7</f>
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="H7">
         <f>[2]npv!H7</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I7">
         <f>[2]npv!I7</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J7">
         <f>[2]npv!J7</f>
@@ -5362,15 +5362,15 @@
       </c>
       <c r="Q7">
         <f>[2]npv!Q7</f>
-        <v>265.519861278414</v>
+        <v>303.756656725016</v>
       </c>
       <c r="R7">
         <f>[2]npv!R7</f>
-        <v>121.272319063518</v>
+        <v>161.852752007102</v>
       </c>
       <c r="S7">
         <f>[2]npv!S7</f>
-        <v>334.51163931970399</v>
+        <v>361.98048738142001</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -5388,27 +5388,27 @@
       </c>
       <c r="D8">
         <f>[2]npv!D8</f>
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="E8">
         <f>[2]npv!E8</f>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F8">
         <f>[2]npv!F8</f>
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="G8">
         <f>[2]npv!G8</f>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H8">
         <f>[2]npv!H8</f>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="I8">
         <f>[2]npv!I8</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J8">
         <f>[2]npv!J8</f>
@@ -5436,19 +5436,19 @@
       </c>
       <c r="P8">
         <f>[2]npv!P8</f>
-        <v>173.34613088085499</v>
+        <v>61.998917149226799</v>
       </c>
       <c r="Q8">
         <f>[2]npv!Q8</f>
-        <v>73.385044698573594</v>
+        <v>35.145553343478603</v>
       </c>
       <c r="R8">
         <f>[2]npv!R8</f>
-        <v>34.252553436585998</v>
+        <v>22.3846643508112</v>
       </c>
       <c r="S8">
         <f>[2]npv!S8</f>
-        <v>91.633623174662006</v>
+        <v>39.373295787402803</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -5474,19 +5474,19 @@
       </c>
       <c r="F9">
         <f>[2]npv!F9</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G9">
         <f>[2]npv!G9</f>
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="H9">
         <f>[2]npv!H9</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="I9">
         <f>[2]npv!I9</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J9">
         <f>[2]npv!J9</f>
@@ -5518,15 +5518,15 @@
       </c>
       <c r="Q9">
         <f>[2]npv!Q9</f>
-        <v>2172.7601582288598</v>
+        <v>2471.34071290063</v>
       </c>
       <c r="R9">
         <f>[2]npv!R9</f>
-        <v>1014.1382856726</v>
+        <v>1335.66717251144</v>
       </c>
       <c r="S9">
         <f>[2]npv!S9</f>
-        <v>2713.05804072</v>
+        <v>2928.94892864036</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -5544,27 +5544,27 @@
       </c>
       <c r="D10">
         <f>[2]npv!D10</f>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <f>[2]npv!E10</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <f>[2]npv!F10</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <f>[2]npv!G10</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="H10">
         <f>[2]npv!H10</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="I10">
         <f>[2]npv!I10</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J10">
         <f>[2]npv!J10</f>
@@ -5592,19 +5592,19 @@
       </c>
       <c r="P10">
         <f>[2]npv!P10</f>
-        <v>-5.2978102793225803</v>
+        <v>-2.0433794339765101</v>
       </c>
       <c r="Q10">
         <f>[2]npv!Q10</f>
-        <v>-2.88427463790243</v>
+        <v>-1.33655007002237</v>
       </c>
       <c r="R10">
         <f>[2]npv!R10</f>
-        <v>-1.7598624002953001</v>
+        <v>-0.98313538804530498</v>
       </c>
       <c r="S10">
         <f>[2]npv!S10</f>
-        <v>-3.2710116590463398</v>
+        <v>-1.44257447461549</v>
       </c>
     </row>
     <row r="11" spans="1:19">
@@ -5630,19 +5630,19 @@
       </c>
       <c r="F11">
         <f>[2]npv!F11</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G11">
         <f>[2]npv!G11</f>
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="H11">
         <f>[2]npv!H11</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I11">
         <f>[2]npv!I11</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J11">
         <f>[2]npv!J11</f>
@@ -5674,15 +5674,15 @@
       </c>
       <c r="Q11">
         <f>[2]npv!Q11</f>
-        <v>189.41567584440099</v>
+        <v>206.469556484902</v>
       </c>
       <c r="R11">
         <f>[2]npv!R11</f>
-        <v>88.409983059034801</v>
+        <v>106.31643073057</v>
       </c>
       <c r="S11">
         <f>[2]npv!S11</f>
-        <v>236.517463946399</v>
+        <v>248.71095050406001</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -5704,23 +5704,23 @@
       </c>
       <c r="E12">
         <f>[2]npv!E12</f>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F12">
         <f>[2]npv!F12</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G12">
         <f>[2]npv!G12</f>
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="H12">
         <f>[2]npv!H12</f>
-        <v>-5</v>
+        <v>8</v>
       </c>
       <c r="I12">
         <f>[2]npv!I12</f>
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="J12">
         <f>[2]npv!J12</f>
@@ -5748,19 +5748,19 @@
       </c>
       <c r="P12">
         <f>[2]npv!P12</f>
-        <v>553.953778990302</v>
+        <v>358.53431254889699</v>
       </c>
       <c r="Q12">
         <f>[2]npv!Q12</f>
-        <v>98.076141206822598</v>
+        <v>134.33185323863401</v>
       </c>
       <c r="R12">
         <f>[2]npv!R12</f>
-        <v>21.0144291894979</v>
+        <v>46.615537998802701</v>
       </c>
       <c r="S12">
         <f>[2]npv!S12</f>
-        <v>211.72091893666899</v>
+        <v>175.27769645976301</v>
       </c>
     </row>
     <row r="13" spans="1:19">
@@ -5778,27 +5778,27 @@
       </c>
       <c r="D13">
         <f>[2]npv!D13</f>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E13">
         <f>[2]npv!E13</f>
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F13">
         <f>[2]npv!F13</f>
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="G13">
         <f>[2]npv!G13</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H13">
         <f>[2]npv!H13</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I13">
         <f>[2]npv!I13</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J13">
         <f>[2]npv!J13</f>
@@ -5826,19 +5826,19 @@
       </c>
       <c r="P13">
         <f>[2]npv!P13</f>
-        <v>380.44106600400198</v>
+        <v>171.70157231237999</v>
       </c>
       <c r="Q13">
         <f>[2]npv!Q13</f>
-        <v>161.05744323226699</v>
+        <v>88.8819648768349</v>
       </c>
       <c r="R13">
         <f>[2]npv!R13</f>
-        <v>75.173745595339298</v>
+        <v>51.535159307582497</v>
       </c>
       <c r="S13">
         <f>[2]npv!S13</f>
-        <v>201.10742077270899</v>
+        <v>102.523805436722</v>
       </c>
     </row>
     <row r="14" spans="1:19">
@@ -5856,27 +5856,27 @@
       </c>
       <c r="D14">
         <f>[2]npv!D14</f>
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="E14">
         <f>[2]npv!E14</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F14">
         <f>[2]npv!F14</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G14">
         <f>[2]npv!G14</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H14">
         <f>[2]npv!H14</f>
-        <v>-5</v>
+        <v>5</v>
       </c>
       <c r="I14">
         <f>[2]npv!I14</f>
-        <v>-5</v>
+        <v>2</v>
       </c>
       <c r="J14">
         <f>[2]npv!J14</f>
@@ -5904,19 +5904,19 @@
       </c>
       <c r="P14">
         <f>[2]npv!P14</f>
-        <v>32.639678313274899</v>
+        <v>15.000809409011699</v>
       </c>
       <c r="Q14">
         <f>[2]npv!Q14</f>
-        <v>7.7790622461947203</v>
+        <v>7.7652254260675599</v>
       </c>
       <c r="R14">
         <f>[2]npv!R14</f>
-        <v>1.91307828755934</v>
+        <v>4.5023996706893303</v>
       </c>
       <c r="S14">
         <f>[2]npv!S14</f>
-        <v>13.4774518787281</v>
+        <v>8.9570528943373393</v>
       </c>
     </row>
     <row r="15" spans="1:19">
@@ -5934,27 +5934,27 @@
       </c>
       <c r="D15">
         <f>[2]npv!D15</f>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E15">
         <f>[2]npv!E15</f>
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F15">
         <f>[2]npv!F15</f>
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="G15">
         <f>[2]npv!G15</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H15">
         <f>[2]npv!H15</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I15">
         <f>[2]npv!I15</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J15">
         <f>[2]npv!J15</f>
@@ -5982,19 +5982,19 @@
       </c>
       <c r="P15">
         <f>[2]npv!P15</f>
-        <v>404.98565090748502</v>
+        <v>182.779093106727</v>
       </c>
       <c r="Q15">
         <f>[2]npv!Q15</f>
-        <v>171.44824602144601</v>
+        <v>94.616285191469402</v>
       </c>
       <c r="R15">
         <f>[2]npv!R15</f>
-        <v>80.023664666006297</v>
+        <v>54.860008295168399</v>
       </c>
       <c r="S15">
         <f>[2]npv!S15</f>
-        <v>214.08209308062601</v>
+        <v>109.13824449715599</v>
       </c>
     </row>
     <row r="16" spans="1:19">
@@ -6012,27 +6012,27 @@
       </c>
       <c r="D16">
         <f>[2]npv!D16</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E16">
         <f>[2]npv!E16</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F16">
         <f>[2]npv!F16</f>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G16">
         <f>[2]npv!G16</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H16">
         <f>[2]npv!H16</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I16">
         <f>[2]npv!I16</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J16">
         <f>[2]npv!J16</f>
@@ -6060,19 +6060,19 @@
       </c>
       <c r="P16">
         <f>[2]npv!P16</f>
-        <v>236.75297521485601</v>
+        <v>153.233118776233</v>
       </c>
       <c r="Q16">
         <f>[2]npv!Q16</f>
-        <v>100.22795190395099</v>
+        <v>76.033849770606807</v>
       </c>
       <c r="R16">
         <f>[2]npv!R16</f>
-        <v>46.781511035809203</v>
+        <v>42.605288494389399</v>
       </c>
       <c r="S16">
         <f>[2]npv!S16</f>
-        <v>125.15152663678001</v>
+        <v>89.165062089429696</v>
       </c>
     </row>
     <row r="17" spans="1:19">
@@ -6094,15 +6094,15 @@
       </c>
       <c r="E17">
         <f>[2]npv!E17</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17">
         <f>[2]npv!F17</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G17">
         <f>[2]npv!G17</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H17">
         <f>[2]npv!H17</f>
@@ -6138,7 +6138,7 @@
       </c>
       <c r="P17">
         <f>[2]npv!P17</f>
-        <v>21.812470504449099</v>
+        <v>20.793378457782499</v>
       </c>
       <c r="Q17">
         <f>[2]npv!Q17</f>
@@ -6150,7 +6150,7 @@
       </c>
       <c r="S17">
         <f>[2]npv!S17</f>
-        <v>13.3955877215149</v>
+        <v>13.0898601075149</v>
       </c>
     </row>
     <row r="18" spans="1:19">
@@ -6168,27 +6168,27 @@
       </c>
       <c r="D18">
         <f>[2]npv!D18</f>
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E18">
         <f>[2]npv!E18</f>
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F18">
         <f>[2]npv!F18</f>
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="G18">
         <f>[2]npv!G18</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H18">
         <f>[2]npv!H18</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I18">
         <f>[2]npv!I18</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J18">
         <f>[2]npv!J18</f>
@@ -6216,19 +6216,19 @@
       </c>
       <c r="P18">
         <f>[2]npv!P18</f>
-        <v>909.23203828066505</v>
+        <v>511.66343592989801</v>
       </c>
       <c r="Q18">
         <f>[2]npv!Q18</f>
-        <v>383.50175019474602</v>
+        <v>264.96792059043599</v>
       </c>
       <c r="R18">
         <f>[2]npv!R18</f>
-        <v>178.28100586497601</v>
+        <v>154.57697883830301</v>
       </c>
       <c r="S18">
         <f>[2]npv!S18</f>
-        <v>479.654613321591</v>
+        <v>305.85929266663499</v>
       </c>
     </row>
     <row r="19" spans="1:19">
@@ -6250,23 +6250,23 @@
       </c>
       <c r="E19">
         <f>[2]npv!E19</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F19">
         <f>[2]npv!F19</f>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G19">
         <f>[2]npv!G19</f>
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="H19">
         <f>[2]npv!H19</f>
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="I19">
         <f>[2]npv!I19</f>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="J19">
         <f>[2]npv!J19</f>
@@ -6294,19 +6294,19 @@
       </c>
       <c r="P19">
         <f>[2]npv!P19</f>
-        <v>427.70336174302798</v>
+        <v>529.12671886748706</v>
       </c>
       <c r="Q19">
         <f>[2]npv!Q19</f>
-        <v>160.92827145451801</v>
+        <v>247.75816005735601</v>
       </c>
       <c r="R19">
         <f>[2]npv!R19</f>
-        <v>68.909266795727703</v>
+        <v>129.53500014332499</v>
       </c>
       <c r="S19">
         <f>[2]npv!S19</f>
-        <v>213.35509714343399</v>
+        <v>296.70177972618598</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved banks to dividends. Changed financials to insurance companies Added forex conversion to prices Cleaned folder
</commit_message>
<xml_diff>
--- a/dashboards/Dashboard_CashFlow.xlsx
+++ b/dashboards/Dashboard_CashFlow.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/telamon/DataScience/repositories/investing/dashboards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BADEAF-4F4A-4646-ADB1-8161EE368B13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28293EB3-0AED-054B-A871-A13408F87D01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="3660" windowWidth="28040" windowHeight="16100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="2" r:id="rId1"/>
-    <sheet name="Price" sheetId="4" r:id="rId2"/>
-    <sheet name="NPV" sheetId="5" r:id="rId3"/>
+    <sheet name="forex" sheetId="6" r:id="rId2"/>
+    <sheet name="Price" sheetId="4" r:id="rId3"/>
+    <sheet name="NPV" sheetId="5" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Master!$A$1:$C$38</definedName>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Ticker</t>
   </si>
@@ -47,6 +48,36 @@
   </si>
   <si>
     <t>Price</t>
+  </si>
+  <si>
+    <t>AAL.L</t>
+  </si>
+  <si>
+    <t>GBP</t>
+  </si>
+  <si>
+    <t>ALA.TO</t>
+  </si>
+  <si>
+    <t>CAD</t>
+  </si>
+  <si>
+    <t>BP.L</t>
+  </si>
+  <si>
+    <t>BTB-UN.TO</t>
+  </si>
+  <si>
+    <t>GLEN.L</t>
+  </si>
+  <si>
+    <t>IAG.L</t>
+  </si>
+  <si>
+    <t>NFI.TO</t>
+  </si>
+  <si>
+    <t>PENCE</t>
   </si>
 </sst>
 </file>
@@ -2711,7 +2742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
@@ -3957,6 +3988,80 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C32FF6B-95FA-834C-9E15-4B0CB838C76E}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{751F6B45-0C58-8944-98B3-2DECD955E5A1}">
   <dimension ref="A1:D47"/>
   <sheetViews>
@@ -4817,7 +4922,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A7F1737-D837-3F4B-A0D1-B5F78C88F34D}">
   <dimension ref="A1:S19"/>
   <sheetViews>

</xml_diff>